<commit_message>
updated package.json and shrinkwrap.json
</commit_message>
<xml_diff>
--- a/stack.xlsx
+++ b/stack.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995" tabRatio="766" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995" tabRatio="766" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="home" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="206">
   <si>
     <t>ReactJs</t>
   </si>
@@ -943,6 +943,24 @@
   </si>
   <si>
     <t>There is also bundledDependencies which is discussed on the following question: Advantages of bundledDependencies over normal dependencies in NPM</t>
+  </si>
+  <si>
+    <t>dev depencies</t>
+  </si>
+  <si>
+    <t>dependencies</t>
+  </si>
+  <si>
+    <t>classnames</t>
+  </si>
+  <si>
+    <t>bodyparser</t>
+  </si>
+  <si>
+    <t>cookie-parser</t>
+  </si>
+  <si>
+    <t>ejs</t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1743,17 +1761,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D21"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="7"/>
-    <col min="2" max="2" width="25.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="91.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" customWidth="1"/>
     <col min="4" max="4" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1853,7 +1871,35 @@
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3">
-      <c r="C21" s="9"/>
+      <c r="B21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>